<commit_message>
1D Lateral interactios implemented, first iteration, by Sebastian Westermann
</commit_message>
<xml_diff>
--- a/results/Finse_4432/CONSTANTS_excel.xlsx
+++ b/results/Finse_4432/CONSTANTS_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\CryoGrid2020_18\results\Finse_4432\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\work\CryoGrid2020_27\results\Finse_4432\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>CONST</t>
   </si>
@@ -255,6 +255,36 @@
   </si>
   <si>
     <t>used in Carman Kozeny model</t>
+  </si>
+  <si>
+    <t>alpha_water</t>
+  </si>
+  <si>
+    <t>alpha_clay</t>
+  </si>
+  <si>
+    <t>alpha_peat</t>
+  </si>
+  <si>
+    <t>from Hydraulic properties of fen peat soils in Poland, Gnatowski 2010</t>
+  </si>
+  <si>
+    <t>n_water</t>
+  </si>
+  <si>
+    <t>n_clay</t>
+  </si>
+  <si>
+    <t>n_peat</t>
+  </si>
+  <si>
+    <t>residual_wc_water</t>
+  </si>
+  <si>
+    <t>residual_wc_clay</t>
+  </si>
+  <si>
+    <t>residual_wc_peat</t>
   </si>
 </sst>
 </file>
@@ -578,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,22 +620,22 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -620,7 +650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -635,7 +665,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -649,7 +679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -663,7 +693,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -677,7 +707,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -691,7 +721,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -704,8 +737,9 @@
       <c r="D13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -719,7 +753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -732,8 +766,9 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -746,16 +781,18 @@
       <c r="D16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -768,8 +805,9 @@
       <c r="D18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -783,7 +821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -797,7 +835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -811,7 +849,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -825,7 +863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -839,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -853,7 +891,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -863,8 +901,9 @@
       <c r="C26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -878,7 +917,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -892,7 +931,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -906,7 +945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -920,7 +959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -966,71 +1005,146 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40">
-        <v>0.65</v>
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B42">
-        <v>1.7</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>2.31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B46">
-        <v>0.1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>74</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55">
+        <v>0.1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B56" s="3">
         <v>2.5</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C56" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>